<commit_message>
Updated test scripts, viterbi and mahalanobis distance
</commit_message>
<xml_diff>
--- a/data/Test/viterbiDataset.xlsx
+++ b/data/Test/viterbiDataset.xlsx
@@ -5,18 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/singo/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/singo/Desktop/MarketStates/data/Test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67ED60E7-EF25-544E-BFE2-1C8C738F3274}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C04954B-25CD-D14F-91FA-9763B7930342}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16560" activeTab="1" xr2:uid="{887CEBC5-32CC-7641-B4D1-65D5FE6AD96A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28040" windowHeight="16520" xr2:uid="{887CEBC5-32CC-7641-B4D1-65D5FE6AD96A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Test1" sheetId="1" r:id="rId1"/>
+    <sheet name="Test2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,24 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Time</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>Path</t>
   </si>
   <si>
     <t>Observation</t>
@@ -71,6 +58,12 @@
   </si>
   <si>
     <t>Random seed</t>
+  </si>
+  <si>
+    <t>True path</t>
+  </si>
+  <si>
+    <t>Min value</t>
   </si>
 </sst>
 </file>
@@ -138,6 +131,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF3DE6C0"/>
+      <color rgb="FFFF5841"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -446,252 +445,537 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58AD690A-F935-3845-A105-6500DD89F70B}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1">
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f ca="1">IF(B$1=$F2,$H$2,RANDBETWEEN($H$2+1,$H$2+3))</f>
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <f ca="1">IF(C$1=$F2,$H$2,RANDBETWEEN($H$2+1,$H$2+3))</f>
+        <v>13</v>
+      </c>
+      <c r="D2">
+        <f ca="1">IF(D$1=$F2,$H$2,RANDBETWEEN($H$2+1,$H$2+3))</f>
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <f ca="1">IF(E$1=$F2,$H$2,RANDBETWEEN($H$2+1,$H$2+3))</f>
+        <v>11</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:E21" ca="1" si="0">IF(B$1=$F3,$H$2,RANDBETWEEN($H$2+1,$H$2+3))</f>
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <f t="shared" ref="A4:A21" si="1">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>10</v>
-      </c>
-      <c r="C2">
-        <v>60</v>
-      </c>
-      <c r="D2">
-        <v>70</v>
-      </c>
-      <c r="E2">
-        <v>80</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>50</v>
-      </c>
-      <c r="C3">
-        <v>10</v>
-      </c>
-      <c r="D3">
-        <v>70</v>
-      </c>
-      <c r="E3">
-        <v>80</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>50</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>70</v>
-      </c>
-      <c r="E4">
-        <v>80</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>50</v>
-      </c>
-      <c r="C5">
-        <v>10</v>
-      </c>
-      <c r="D5">
-        <v>70</v>
-      </c>
-      <c r="E5">
-        <v>80</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6">
-        <v>5</v>
-      </c>
       <c r="B6">
-        <v>50</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
       </c>
       <c r="C6">
-        <v>60</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
       </c>
       <c r="D6">
+        <f t="shared" ca="1" si="0"/>
         <v>10</v>
       </c>
       <c r="E6">
-        <v>80</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
       </c>
       <c r="F6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:8">
       <c r="A7">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B7">
-        <v>50</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
       </c>
       <c r="C7">
-        <v>60</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
       </c>
       <c r="D7">
+        <f t="shared" ca="1" si="0"/>
         <v>10</v>
       </c>
       <c r="E7">
-        <v>80</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
       </c>
       <c r="F7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:8">
       <c r="A8">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B8">
-        <v>50</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
       </c>
       <c r="C8">
-        <v>60</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
       </c>
       <c r="D8">
-        <v>10</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
       </c>
       <c r="E8">
-        <v>80</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
       </c>
       <c r="F8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B9">
-        <v>50</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
       </c>
       <c r="C9">
-        <v>60</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
       </c>
       <c r="D9">
-        <v>70</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
       </c>
       <c r="E9">
+        <f t="shared" ca="1" si="0"/>
         <v>10</v>
       </c>
       <c r="F9">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:8">
       <c r="A10">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B10">
-        <v>50</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
       </c>
       <c r="C10">
-        <v>60</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
       </c>
       <c r="D10">
-        <v>70</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
       </c>
       <c r="E10">
-        <v>10</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
       </c>
       <c r="F10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="E16">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F16">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>50</v>
-      </c>
-      <c r="C11">
-        <v>60</v>
-      </c>
-      <c r="D11">
-        <v>70</v>
-      </c>
-      <c r="E11">
-        <v>10</v>
-      </c>
-      <c r="F11">
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F17">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>50</v>
-      </c>
-      <c r="C12">
-        <v>60</v>
-      </c>
-      <c r="D12">
-        <v>70</v>
-      </c>
-      <c r="E12">
-        <v>10</v>
-      </c>
-      <c r="F12">
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="E18">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F18">
         <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C19">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C20">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="F20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F21">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -703,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{953CD5C9-87F0-084A-9CB5-34782A31679F}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10:R11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -719,25 +1003,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -746,18 +1030,18 @@
       </c>
       <c r="B2" s="4">
         <f ca="1">RAND()</f>
-        <v>0.67229299391695951</v>
+        <v>0.63127243570140334</v>
       </c>
       <c r="C2" s="4">
         <f ca="1">_xlfn.NORM.INV(B2,IF(D2=$F$2,$G$2,$G$3),IF(D2=$F$2,$H$2,$H$3))</f>
-        <v>0.94625367873629562</v>
+        <v>0.83522531303791081</v>
       </c>
       <c r="D2" s="4">
         <v>1</v>
       </c>
       <c r="E2" s="4">
         <f ca="1">(C2-$G$2)^2/$H$2</f>
-        <v>0.19914234578567694</v>
+        <v>0.11237601050136529</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
@@ -775,18 +1059,18 @@
       </c>
       <c r="B3" s="4">
         <f t="shared" ref="B3:B21" ca="1" si="0">RAND()</f>
-        <v>0.58928280170769254</v>
+        <v>0.4970738316254526</v>
       </c>
       <c r="C3" s="4">
         <f t="shared" ref="C3:C21" ca="1" si="1">_xlfn.NORM.INV(B3,IF(D3=$F$2,$G$2,$G$3),IF(D3=$F$2,$H$2,$H$3))</f>
-        <v>0.7257004647623666</v>
+        <v>0.49266511784650929</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
       </c>
       <c r="E3" s="4">
         <f t="shared" ref="E3:E10" ca="1" si="2">(C3-$G$2)^2/$H$2</f>
-        <v>5.0940699793948288E-2</v>
+        <v>5.3800496205596475E-5</v>
       </c>
       <c r="F3" s="2">
         <v>2</v>
@@ -804,18 +1088,18 @@
       </c>
       <c r="B4" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.94234034722082272</v>
+        <v>0.96808327979243292</v>
       </c>
       <c r="C4" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>2.0747277242128455</v>
+        <v>2.3533414026205257</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>2.4797674054045675</v>
+        <v>3.4348743546674174</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -824,18 +1108,18 @@
       </c>
       <c r="B5" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.38723739607682461</v>
+        <v>0.83419647324831925</v>
       </c>
       <c r="C5" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.21347335941877366</v>
+        <v>1.4708819781374682</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>8.2097515762763265E-2</v>
+        <v>0.94261181547212336</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -844,18 +1128,18 @@
       </c>
       <c r="B6" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.27032718476293627</v>
+        <v>0.72497296864567262</v>
       </c>
       <c r="C6" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.11182375742841355</v>
+        <v>1.0976791162234614</v>
       </c>
       <c r="D6" s="4">
         <v>1</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>0.37432831015382223</v>
+        <v>0.35722032596965786</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -864,18 +1148,18 @@
       </c>
       <c r="B7" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.60335955653974793</v>
+        <v>0.14019989928665999</v>
       </c>
       <c r="C7" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.76205260367277239</v>
+        <v>-0.57942166198805767</v>
       </c>
       <c r="D7" s="4">
         <v>1</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>6.8671567091679125E-2</v>
+        <v>1.1651511243690607</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -884,18 +1168,18 @@
       </c>
       <c r="B8" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.9667917680957907</v>
+        <v>0.45318182323512224</v>
       </c>
       <c r="C8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>2.3356025226231374</v>
+        <v>0.38237355013740992</v>
       </c>
       <c r="D8" s="4">
         <v>1</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>3.3694366210604256</v>
+        <v>1.3835981707276417E-2</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -904,18 +1188,18 @@
       </c>
       <c r="B9" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.63602507350808801</v>
+        <v>0.18628700893041661</v>
       </c>
       <c r="C9" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.84785397334856727</v>
+        <v>-0.39166220411636277</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>0.12100238677438575</v>
+        <v>0.79506148624965023</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -924,18 +1208,18 @@
       </c>
       <c r="B10" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.67492910045107202</v>
+        <v>0.96431523313667977</v>
       </c>
       <c r="C10" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.9535652090310669</v>
+        <v>2.3031189623927775</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>0.20572139884339541</v>
+        <v>3.2512379925404065</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -944,18 +1228,18 @@
       </c>
       <c r="B11" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>3.0232462179099917E-2</v>
+        <v>0.14025997262830647</v>
       </c>
       <c r="C11" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.3773880775066385</v>
+        <v>-0.57915206322926926</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
       </c>
       <c r="E11" s="4">
         <f ca="1">(C11-$G$2)^2/$H$2</f>
-        <v>3.524585993564072</v>
+        <v>1.1645691755719887</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -964,18 +1248,18 @@
       </c>
       <c r="B12" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.49193702767036362</v>
+        <v>0.78531552714923458</v>
       </c>
       <c r="C12" s="4">
         <f ca="1">_xlfn.NORM.INV(B12,IF(D12=$F$2,$G$2,$G$3),IF(D12=$F$2,$H$2,$H$3))</f>
-        <v>-0.42021225057024608</v>
+        <v>0.39027198225200732</v>
       </c>
       <c r="D12" s="4">
         <v>2</v>
       </c>
       <c r="E12" s="4">
         <f ca="1">(C12-$G$3)^2/$H$3</f>
-        <v>4.0853507311441217E-4</v>
+        <v>0.62452980593251706</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -984,18 +1268,18 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>6.9100203213897093E-2</v>
+        <v>0.51213590969104794</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.8825259409961017</v>
+        <v>-0.36957509235231201</v>
       </c>
       <c r="D13" s="4">
         <v>2</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" ref="E13:E21" ca="1" si="3">(C13-$G$3)^2/$H$3</f>
-        <v>2.1978831657263771</v>
+        <v>9.2567500537034473E-4</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1004,18 +1288,18 @@
       </c>
       <c r="B14" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.31706931639464586</v>
+        <v>0.76965719608864636</v>
       </c>
       <c r="C14" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.87590981026120862</v>
+        <v>0.33771836818571488</v>
       </c>
       <c r="D14" s="4">
         <v>2</v>
       </c>
       <c r="E14" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>0.22649014750285956</v>
+        <v>0.54422839075859397</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1024,18 +1308,18 @@
       </c>
       <c r="B15" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.88792481139866586</v>
+        <v>1.628772579044846E-2</v>
       </c>
       <c r="C15" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.81556577806129382</v>
+        <v>-2.5372772072144327</v>
       </c>
       <c r="D15" s="4">
         <v>2</v>
       </c>
       <c r="E15" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>1.4776001607937588</v>
+        <v>4.5679538604783252</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1044,18 +1328,18 @@
       </c>
       <c r="B16" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.54044654074505605</v>
+        <v>0.45488742822222039</v>
       </c>
       <c r="C16" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.29844124456654131</v>
+        <v>-0.51332252935806522</v>
       </c>
       <c r="D16" s="4">
         <v>2</v>
       </c>
       <c r="E16" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>1.031418080519308E-2</v>
+        <v>1.2841995660109547E-2</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1064,18 +1348,18 @@
       </c>
       <c r="B17" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.87057047796654485</v>
+        <v>0.77324955735424628</v>
       </c>
       <c r="C17" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.72909195655230585</v>
+        <v>0.34959131148923306</v>
       </c>
       <c r="D17" s="4">
         <v>2</v>
       </c>
       <c r="E17" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>1.2748486463511142</v>
+        <v>0.56188713426014847</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1084,18 +1368,18 @@
       </c>
       <c r="B18" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15607897329982734</v>
+        <v>0.77910078487968037</v>
       </c>
       <c r="C18" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.4107043663814061</v>
+        <v>0.36915983616620707</v>
       </c>
       <c r="D18" s="4">
         <v>2</v>
       </c>
       <c r="E18" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>1.0215233162224397</v>
+        <v>0.59160685357122655</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1104,18 +1388,18 @@
       </c>
       <c r="B19" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.53078334891713119</v>
+        <v>0.29031717873771234</v>
       </c>
       <c r="C19" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.322760855914621</v>
+        <v>-0.95245835751743146</v>
       </c>
       <c r="D19" s="4">
         <v>2</v>
       </c>
       <c r="E19" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>5.9658853790419408E-3</v>
+        <v>0.30521023679085812</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1124,18 +1408,18 @@
       </c>
       <c r="B20" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.48961908311071245</v>
+        <v>3.2601937833356631E-2</v>
       </c>
       <c r="C20" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.42602403695823537</v>
+        <v>-2.2438577373810578</v>
       </c>
       <c r="D20" s="4">
         <v>2</v>
       </c>
       <c r="E20" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>6.7725049960359949E-4</v>
+        <v>3.399811355699994</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1144,18 +1428,18 @@
       </c>
       <c r="B21" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1937158795253597E-2</v>
+        <v>0.93364248363243174</v>
       </c>
       <c r="C21" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.4152895655989819</v>
+        <v>1.1034810781601654</v>
       </c>
       <c r="D21" s="4">
         <v>2</v>
       </c>
       <c r="E21" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>4.0613920332121332</v>
+        <v>2.260455352385653</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1168,4 +1452,28 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB6043F-755D-4D49-855C-0BAA7F53463B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4B2ABA8-3C14-3B48-ADD6-836B41232CDF}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>